<commit_message>
Add CVC import option to credit card importer
</commit_message>
<xml_diff>
--- a/templates/Untokenized Credit Cards.xlsx
+++ b/templates/Untokenized Credit Cards.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -117,12 +117,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The CVC code is the 3 or 4 digit code on the back of a credit card. If your payment processor does not require the CVC for tokenization, this can be excluded. If they require it, it must be included.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Account ID</t>
   </si>
@@ -155,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVC</t>
   </si>
 </sst>
 </file>
@@ -188,6 +204,7 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
     </font>
@@ -199,7 +216,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +227,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5E8AC7"/>
+        <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
   </fills>
@@ -247,12 +270,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -282,7 +309,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF5E8AC7"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -339,9 +366,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>742320</xdr:colOff>
+      <xdr:colOff>741960</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -351,7 +378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="30240" y="0"/>
-          <a:ext cx="5512680" cy="5344920"/>
+          <a:ext cx="5512320" cy="5344560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -372,69 +399,50 @@
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>This import can be used to insert raw (untokenized) credit card data into Sonar. Be mindful of security and your PCI compliance obligations if using this import!</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>Grey columns are required, blue columns are optional.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -452,18 +460,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.34"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -477,22 +485,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,11 +537,14 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>